<commit_message>
Edit FirstNamr and lastname from username
</commit_message>
<xml_diff>
--- a/children.xlsx
+++ b/children.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\marmina\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ADFC3D-0E51-44FB-885C-E331EDCA7F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C88F06-B494-434B-ACFF-2A12FAB8154A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>name</t>
   </si>
@@ -57,37 +57,10 @@
     <t>20 شارع النزهه</t>
   </si>
   <si>
-    <t>21 شارع النزهه</t>
-  </si>
-  <si>
-    <t>22 شارع النزهه</t>
-  </si>
-  <si>
-    <t>23 شارع النزهه</t>
-  </si>
-  <si>
     <t>ابونا ابامون</t>
   </si>
   <si>
-    <t>ابونا اباهور</t>
-  </si>
-  <si>
-    <t>ابونا سرجيوس</t>
-  </si>
-  <si>
-    <t>ابونا صرابامون</t>
-  </si>
-  <si>
     <t>Anton Nashaat</t>
-  </si>
-  <si>
-    <t>Ramy Ayman</t>
-  </si>
-  <si>
-    <t>Toto Kaboto</t>
-  </si>
-  <si>
-    <t>Chafe Inesta</t>
   </si>
 </sst>
 </file>
@@ -412,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,7 +435,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>39083</v>
@@ -477,91 +450,13 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1">
         <v>39814</v>
       </c>
       <c r="I2">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1">
-        <v>39084</v>
-      </c>
-      <c r="C3">
-        <v>1254477831</v>
-      </c>
-      <c r="D3">
-        <v>1254478963</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1">
-        <v>39815</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1">
-        <v>39085</v>
-      </c>
-      <c r="C4">
-        <v>1254477963</v>
-      </c>
-      <c r="D4">
-        <v>1254477963</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1">
-        <v>39816</v>
-      </c>
-      <c r="I4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1">
-        <v>39086</v>
-      </c>
-      <c r="C5">
-        <v>1248541471</v>
-      </c>
-      <c r="D5">
-        <v>1248541471</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1">
-        <v>39817</v>
-      </c>
-      <c r="I5">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>